<commit_message>
para fazer em casa
</commit_message>
<xml_diff>
--- a/db/Encomendas.xlsx
+++ b/db/Encomendas.xlsx
@@ -348,7 +348,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -531,7 +531,7 @@
         </is>
       </c>
       <c r="B5" s="1" t="n">
-        <v>43594.6468402738</v>
+        <v>43594.64684027381</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -564,6 +564,48 @@
       </c>
       <c r="J5" t="n">
         <v>8.800000000000001</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Brevemente</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>44145.65398057337</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>dadadada</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Produtos para Gatos</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>3</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fabricante: ROYAL CANIN AROMATIC EXIGENT; </t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" t="n">
+        <v>4.78</v>
+      </c>
+      <c r="J6" t="n">
+        <v>4.78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>